<commit_message>
edits to dickson protocol, wait 90 secs before starting experiment
</commit_message>
<xml_diff>
--- a/ProtocolFiles/EP_Bubble_v001p1.xlsx
+++ b/ProtocolFiles/EP_Bubble_v001p1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>CV term</t>
   </si>
@@ -65,7 +65,7 @@
     <t>gender</t>
   </si>
   <si>
-    <t>b</t>
+    <t>m or f</t>
   </si>
   <si>
     <t>string</t>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>4 flybubble rigs arrowroot, beet, carrot, daikon</t>
+  </si>
+  <si>
+    <t>overhead lights off, screns dimmed with red channel lowered</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -428,7 +431,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
@@ -569,7 +572,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="8" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>5</v>
@@ -597,7 +600,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="15" t="n">
-        <v>20150330</v>
+        <v>20180315</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>37</v>
@@ -629,6 +632,13 @@
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
+    </row>
+    <row r="19" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>